<commit_message>
Adding .docx file generation feature
</commit_message>
<xml_diff>
--- a/data/discussions_history.xlsx
+++ b/data/discussions_history.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://bayergroup-my.sharepoint.com/personal/axel_cano_bayer_com/Documents/desktop/Axel/Code/Projets/byr_HSE_subjects/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="62" documentId="11_F25DC773A252ABDACC104855D91F74005BDE58EA" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D6FDC43E-8ADC-410F-8C1A-4742A707C897}"/>
+  <xr:revisionPtr revIDLastSave="63" documentId="11_F25DC773A252ABDACC104855D91F74005BDE58EA" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5DE6C24F-4C6C-4CCF-A67A-65D538CB0B8D}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -493,7 +493,8 @@
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="24.7109375" style="1" customWidth="1"/>
-    <col min="2" max="16384" width="9.140625" style="1"/>
+    <col min="2" max="2" width="14.7109375" style="1" customWidth="1"/>
+    <col min="3" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">

</xml_diff>